<commit_message>
adding adress book example
</commit_message>
<xml_diff>
--- a/examples/children_fav_games/schema_and_data.xlsx
+++ b/examples/children_fav_games/schema_and_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="28800" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,11 @@
     <sheet name="!!Parent" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$3:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!_Schema'!$A$2:$G$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$3:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Child'!$A$3:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -32,9 +32,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.
@@ -47,9 +46,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
@@ -61,9 +59,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Select one of "female", "male".</t>
         </r>
@@ -74,9 +71,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a comma-separated list of values from "Parent:1" or blank.</t>
         </r>
@@ -87,9 +83,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.
@@ -102,9 +97,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
@@ -116,9 +110,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter an integer.</t>
         </r>
@@ -139,9 +132,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.
@@ -154,9 +146,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
@@ -168,16 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
-  <si>
-    <t>'!!_Schema'!A1</t>
-  </si>
-  <si>
-    <t>'!!Child'!A1</t>
-  </si>
-  <si>
-    <t>'!!Parent'!A1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8' date='2020-03-14 11:51:05'</t>
   </si>
@@ -393,35 +375,191 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +580,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="65"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,8 +590,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -460,35 +785,328 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -771,636 +1389,653 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="3" width="15.7133333333333" customWidth="1"/>
+    <col min="4" max="16384" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" customHeight="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="4" customHeight="1" spans="1:3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:3">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A3:C6"/>
+  <sheetProtection sheet="1" insertRows="0" deleteRows="0" objects="1" scenarios="1"/>
+  <autoFilter ref="A3:C6">
+    <extLst/>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="A4" location="'!!_Schema'!A1" tooltip="Click to view schema" display="'!!_Schema'!A1"/>
-    <hyperlink ref="A5" location="'!!Child'!A1" tooltip="Click to view child" display="'!!Child'!A1"/>
-    <hyperlink ref="A6" location="'!!Parent'!A1" tooltip="Click to view parent" display="'!!Parent'!A1"/>
+    <hyperlink ref="A4" location="'!!_Schema'!A1" display="Schema" tooltip="Click to view schema"/>
+    <hyperlink ref="A5" location="'!!Child'!A1" display="Child" tooltip="Click to view child"/>
+    <hyperlink ref="A6" location="'!!Parent'!A1" display="Parent" tooltip="Click to view parent"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="7" width="15.7133333333333" customWidth="1"/>
+    <col min="8" max="16384" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" customHeight="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:7">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:7">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" customHeight="1" spans="1:7">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" customHeight="1" spans="1:7">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:7">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:7">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" customHeight="1" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:7">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:7">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" customHeight="1" spans="1:7">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" customHeight="1" spans="1:7">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A2:G15"/>
+  <sheetProtection sheet="1" insertRows="0" deleteRows="0" objects="1" scenarios="1"/>
+  <autoFilter ref="A2:G15">
+    <extLst/>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="A3" location="'!!Child'!A1" tooltip="Click to view child" display="'!!Child'!A1"/>
-    <hyperlink ref="A9" location="'!!Parent'!A1" tooltip="Click to view parent" display="'!!Parent'!A1"/>
+    <hyperlink ref="A3" location="'!!Child'!A1" display="Child" tooltip="Click to view child"/>
+    <hyperlink ref="A9" location="'!!Parent'!A1" display="Parent" tooltip="Click to view parent"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="7" width="15.7133333333333" customWidth="1"/>
+    <col min="8" max="16384" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" customHeight="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:7">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" customHeight="1" spans="1:7">
+      <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G4" s="3">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:7">
+      <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="4">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="F5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:7">
+      <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="4">
-        <v>1985</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="4">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.01" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>1989</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A3:G7"/>
+  <sheetProtection sheet="1" insertRows="0" deleteRows="0" objects="1" scenarios="1"/>
+  <autoFilter ref="A3:G7">
+    <extLst/>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="E2:G2"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A4:A7">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B4:B7" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B4:B7">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Gender" error="Value must be one of &quot;female&quot;, &quot;male&quot;." promptTitle="Gender" prompt="Select one of &quot;female&quot;, &quot;male&quot;." sqref="C4:C7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Parents" error="Value must be a comma-separated list of values from &quot;Parent:1&quot; or blank." promptTitle="Parents" prompt="Enter a comma-separated list of values from &quot;Parent:1&quot; or blank." sqref="D4:D7" errorStyle="warning"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Gender" error="Value must be one of &quot;female&quot;, &quot;male&quot;." promptTitle="Gender" prompt="Select one of &quot;female&quot;, &quot;male&quot;." sqref="C4:C7" errorStyle="warning">
       <formula1>"female,male"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Parents" error="Value must be a comma-separated list of values from &quot;Parent:1&quot; or blank." promptTitle="Parents" prompt="Enter a comma-separated list of values from &quot;Parent:1&quot; or blank." sqref="D4:D7"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="E4:E7">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Publisher" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Publisher" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="F4:F7">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Year" error="Value must be an integer." promptTitle="Year" prompt="Enter an integer." sqref="G4:G7">
+    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Year" error="Value must be an integer." promptTitle="Year" prompt="Enter an integer." sqref="G4:G7" errorStyle="warning">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="E4:E7" errorStyle="warning">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Publisher" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Publisher" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="F4:F7" errorStyle="warning">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A4:A7" errorStyle="warning">
+      <formula1>255</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="5" width="15.7133333333333" customWidth="1"/>
+    <col min="6" max="16384" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" customHeight="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" customHeight="1" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>72</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection sheet="1" insertRows="0" deleteRows="0" objects="1" scenarios="1"/>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="B2:E2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:E3" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:E3">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="B2:E2" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>